<commit_message>
taking comments from Clotaire & Sylvain a6260b2861daf1aeae2ef12ad794a5e55e274243
</commit_message>
<xml_diff>
--- a/ig/ft-3-add-narative/StructureDefinition-cds-ihe-careteam.xlsx
+++ b/ig/ft-3-add-narative/StructureDefinition-cds-ihe-careteam.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-21T15:34:54+00:00</t>
+    <t>2024-03-18T15:36:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1109,7 +1109,7 @@
     <t>CareTeam.participant.member</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-practitionerrole|http://interop.esante.gouv.fr/ig/fhir/cds/StructureDefinition/cds-fr-related-person|https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-organization|http://interop.esante.gouv.fr/ig/fhir/cds/StructureDefinition/cds-organization-interne)
+    <t xml:space="preserve">Reference(https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-practitionerrole|http://interop.esante.gouv.fr/ig/fhir/cds/StructureDefinition/cds-fr-related-person|https://interop.esante.gouv.fr/ig/fhir/annuaire/StructureDefinition/as-organization)
 </t>
   </si>
   <si>
@@ -1605,7 +1605,7 @@
     <col min="8" max="8" width="16.27734375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.26171875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="255.0" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="238.8046875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>